<commit_message>
Added .htaccess in root folder
</commit_message>
<xml_diff>
--- a/storage/files/DTRTemplates/dtrsummary.xlsx
+++ b/storage/files/DTRTemplates/dtrsummary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="19440" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="19440" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,15 +80,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -96,22 +87,39 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -145,28 +153,28 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,53 +458,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="6" customWidth="1"/>
-    <col min="2" max="4" width="13.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="6" customWidth="1"/>
-    <col min="7" max="10" width="13.7109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="7"/>
-    <col min="12" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="18.140625" style="2" customWidth="1"/>
+    <col min="2" max="4" width="13.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="4" customWidth="1"/>
+    <col min="7" max="10" width="13.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="10"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="5" t="s">
+      <c r="L1" s="5"/>
+      <c r="M1" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -509,40 +517,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="10" customWidth="1"/>
-    <col min="4" max="5" width="17.7109375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="3" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="9" customFormat="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>